<commit_message>
h2 with reactive, http api gateway
</commit_message>
<xml_diff>
--- a/docs/HnT 1H&T 5.0 Account specific V2.xlsx
+++ b/docs/HnT 1H&T 5.0 Account specific V2.xlsx
@@ -431,11 +431,14 @@
     <t xml:space="preserve">API Gateway</t>
   </si>
   <si>
-    <t xml:space="preserve">Introduction to Amazon API Gateway | API Gateway use cases - Use API Gateway to create HTTP APIs, REST APIs | Choosing between HTTP APIs and REST API 
-Build an API Gateway REST API with AWS integration
-Create and publish a HTTP API
-Monitor published APIs
-Integrate BE with API Gateway</t>
+    <t xml:space="preserve">Introduction to Amazon API Gateway 
+API Gateway use cases 
+Use API Gateway to create 
+- HTTP APIs
+- REST APIs 
+- Choosing between HTTP APIs and REST API   
+Build an API Gateway REST API with AWS integration 
+Create and publish a HTTP API Monitor published APIs Integrate BE with API Gateway</t>
   </si>
   <si>
     <t xml:space="preserve">Database Basics - slq/no-sql, MongoDB</t>
@@ -582,7 +585,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MMM"/>
+    <numFmt numFmtId="165" formatCode="dd/mmm"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -1119,7 +1122,85 @@
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
     <cellStyle name="Normal 2 2" xfId="20"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="20">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF808080"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="00FFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF000000"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF93CDDD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD7E4BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFD99694"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4F81BD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF558ED5"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1252,21 +1333,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:J44"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B31" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E35" activeCellId="0" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.703125" defaultRowHeight="14.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="11.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="67.45"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="46.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="20.98"/>
@@ -1898,7 +1979,7 @@
       <c r="H32" s="32"/>
       <c r="I32" s="32"/>
     </row>
-    <row r="33" customFormat="false" ht="52.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="74.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="43"/>
       <c r="B33" s="46" t="s">
         <v>71</v>
@@ -2143,37 +2224,37 @@
     <mergeCell ref="D42:E42"/>
   </mergeCells>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>4</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="13">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="14">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="15">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="5">
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="16">
       <formula>"E"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="6">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="17">
       <formula>"S"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="18">
       <formula>"P"</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="8">
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="19">
       <formula>"L"</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>